<commit_message>
Aankomst en Vertrek Depots toegevoegd
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6aaedf7c31cb3db/Documenten/TA_ABMS/code_student_versie10_09/code_student_versie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\AE4422-20_G01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{8619D402-E8AF-48C7-ADA5-03BC2EAEC118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40FE721-0762-4D8D-A5B7-2D189D2270B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FADFD-4EF2-45BA-919B-F03D5F2D2629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
+    <workbookView xWindow="1644" yWindow="3360" windowWidth="17796" windowHeight="8880" xr2:uid="{1DB0F0EF-2216-4628-B5EE-950EADE27966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -101,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +141,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +247,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937278-08B5-42DE-93BA-E4F0710E1C5E}">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="G237" sqref="G237"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E262" sqref="E262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3188,6 +3188,138 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>29</v>
+      </c>
+      <c r="B254">
+        <v>109</v>
+      </c>
+      <c r="C254">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>109</v>
+      </c>
+      <c r="B255">
+        <v>29</v>
+      </c>
+      <c r="C255">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>109</v>
+      </c>
+      <c r="B256">
+        <v>112</v>
+      </c>
+      <c r="C256">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>112</v>
+      </c>
+      <c r="B257">
+        <v>109</v>
+      </c>
+      <c r="C257">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>104</v>
+      </c>
+      <c r="B258">
+        <v>110</v>
+      </c>
+      <c r="C258">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>110</v>
+      </c>
+      <c r="B259">
+        <v>104</v>
+      </c>
+      <c r="C259">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>110</v>
+      </c>
+      <c r="B260">
+        <v>112</v>
+      </c>
+      <c r="C260">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>112</v>
+      </c>
+      <c r="B261">
+        <v>110</v>
+      </c>
+      <c r="C261">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>10</v>
+      </c>
+      <c r="B262">
+        <v>111</v>
+      </c>
+      <c r="C262">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>111</v>
+      </c>
+      <c r="B263">
+        <v>10</v>
+      </c>
+      <c r="C263">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>111</v>
+      </c>
+      <c r="B264">
+        <v>113</v>
+      </c>
+      <c r="C264">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>113</v>
+      </c>
+      <c r="B265">
+        <v>111</v>
+      </c>
+      <c r="C265">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>